<commit_message>
Modified code to work with current Study cases and Experiments
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Study case 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Study case 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Study case 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Study case 4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Experiment 1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Experiment 2" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,11 +449,6 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Manhattan Distance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -461,29 +457,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7505182801979318</v>
+        <v>0.7458308217580214</v>
       </c>
       <c r="C2" t="n">
-        <v>3.95444046567113</v>
-      </c>
-      <c r="D2" t="n">
-        <v>49.71206585278696</v>
+        <v>3.608247796187873</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>pt -&gt; en -&gt; es</t>
+          <t>pt -&gt; it -&gt; es</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7224728153038819</v>
+        <v>0.7253818860884673</v>
       </c>
       <c r="C3" t="n">
-        <v>4.17852961718367</v>
-      </c>
-      <c r="D3" t="n">
-        <v>54.01499439648984</v>
+        <v>3.72803316185625</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,154 +506,31 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Manhattan Distance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>pt -&gt; es</t>
+          <t>en -&gt; sv</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7505182801979318</v>
+        <v>0.770321545661382</v>
       </c>
       <c r="C2" t="n">
-        <v>3.95444046567113</v>
-      </c>
-      <c r="D2" t="n">
-        <v>49.71206585278696</v>
+        <v>4.096113994901942</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>pt -&gt; fr -&gt; es</t>
+          <t>en -&gt; de -&gt; sv</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7347473065759326</v>
+        <v>0.7507004719405196</v>
       </c>
       <c r="C3" t="n">
-        <v>4.06541432466208</v>
-      </c>
-      <c r="D3" t="n">
-        <v>51.72228082095476</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; it -&gt; es</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7364197443155868</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4.045299990304325</v>
-      </c>
-      <c r="D4" t="n">
-        <v>51.27948242497737</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; ro -&gt; es</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7239133136247261</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4.162425719052401</v>
-      </c>
-      <c r="D5" t="n">
-        <v>53.56351030867478</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; fr -&gt; it -&gt; es</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.7247421195038368</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4.12875816120399</v>
-      </c>
-      <c r="D6" t="n">
-        <v>52.80280990766791</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; fr -&gt; ro -&gt; es</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.7134525705055645</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4.216944210791296</v>
-      </c>
-      <c r="D7" t="n">
-        <v>54.35319074329513</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; it -&gt; ro -&gt; es</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.7152516306184843</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.208782419115269</v>
-      </c>
-      <c r="D8" t="n">
-        <v>54.25118914740192</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; fr -&gt; it -&gt; ro -&gt; es</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.7058015953099167</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4.269050061416896</v>
-      </c>
-      <c r="D9" t="n">
-        <v>55.16104682032371</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; fr -&gt; it -&gt; en -&gt; ro -&gt; es</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.6925821399371306</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4.369907669525831</v>
-      </c>
-      <c r="D10" t="n">
-        <v>56.85226267996551</v>
+        <v>4.223161091188399</v>
       </c>
     </row>
   </sheetData>
@@ -677,7 +544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,154 +563,31 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Manhattan Distance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>en -&gt; de</t>
+          <t>pt -&gt; es</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7383752420426122</v>
+        <v>0.7458308217580214</v>
       </c>
       <c r="C2" t="n">
-        <v>4.653678207316533</v>
-      </c>
-      <c r="D2" t="n">
-        <v>60.1311618516932</v>
+        <v>3.608247796187873</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>en -&gt; sv -&gt; de</t>
+          <t>pt -&gt; en -&gt; es</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7262416235619358</v>
+        <v>0.7183457890793921</v>
       </c>
       <c r="C3" t="n">
-        <v>4.735488320271665</v>
-      </c>
-      <c r="D3" t="n">
-        <v>61.69778901423597</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; nl -&gt; de</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7322264082727739</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4.694411613676471</v>
-      </c>
-      <c r="D4" t="n">
-        <v>60.99539927486921</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; da -&gt; de</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7262011603177246</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4.738022385802446</v>
-      </c>
-      <c r="D5" t="n">
-        <v>61.56790602450655</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; sv -&gt; nl -&gt; de</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.7230593194380058</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4.754768383935515</v>
-      </c>
-      <c r="D6" t="n">
-        <v>62.06184071635955</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; sv -&gt; da -&gt; de</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.7177511299705817</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4.790198749760102</v>
-      </c>
-      <c r="D7" t="n">
-        <v>62.52522140159996</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; nl -&gt; da -&gt; de</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.7207250639390482</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.770221322838627</v>
-      </c>
-      <c r="D8" t="n">
-        <v>62.11254245803723</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; sv -&gt; nl -&gt; da -&gt; de</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.7135179633683902</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4.816308990272381</v>
-      </c>
-      <c r="D9" t="n">
-        <v>62.97938042382053</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; sv -&gt; it -&gt; nl -&gt; da -&gt; de</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.7011758079062268</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4.896321189012427</v>
-      </c>
-      <c r="D10" t="n">
-        <v>64.24049318596637</v>
+        <v>3.794852705933903</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +601,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,11 +620,6 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Manhattan Distance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -889,125 +628,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7505182801979318</v>
+        <v>0.7458308217580214</v>
       </c>
       <c r="C2" t="n">
-        <v>3.95444046567113</v>
-      </c>
-      <c r="D2" t="n">
-        <v>49.71206585278696</v>
+        <v>3.608247796187873</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>pt -&gt; de -&gt; es</t>
+          <t>pt -&gt; en -&gt; es</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7139671485691763</v>
+        <v>0.7183457890793921</v>
       </c>
       <c r="C3" t="n">
-        <v>4.244939717767526</v>
-      </c>
-      <c r="D3" t="n">
-        <v>54.84561182523492</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; fr -&gt; es</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7347473065759326</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4.06541432466208</v>
-      </c>
-      <c r="D4" t="n">
-        <v>51.72228082095476</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; en -&gt; es</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7224728153038819</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4.17852961718367</v>
-      </c>
-      <c r="D5" t="n">
-        <v>54.01499439648984</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; de -&gt; fr -&gt; es</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.7069750221705853</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4.279639132034768</v>
-      </c>
-      <c r="D6" t="n">
-        <v>55.45588584202486</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; de -&gt; en -&gt; es</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.6962513380263139</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4.373202082640088</v>
-      </c>
-      <c r="D7" t="n">
-        <v>56.85184644300317</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; fr -&gt; en -&gt; es</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.7104849148673456</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.250460610478521</v>
-      </c>
-      <c r="D8" t="n">
-        <v>55.01911338926997</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>pt -&gt; de -&gt; fr -&gt; en -&gt; es</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.6974954865718779</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4.351857671952988</v>
-      </c>
-      <c r="D9" t="n">
-        <v>56.56627766478109</v>
+        <v>3.794852705933903</v>
       </c>
     </row>
   </sheetData>
@@ -1021,7 +658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1040,138 +677,88 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Manhattan Distance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>en -&gt; de</t>
+          <t>pt -&gt; de</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7383752420426122</v>
+        <v>0.6468203826557445</v>
       </c>
       <c r="C2" t="n">
-        <v>4.653678207316533</v>
-      </c>
-      <c r="D2" t="n">
-        <v>60.1311618516932</v>
+        <v>4.090183607972863</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>en -&gt; es -&gt; de</t>
+          <t>pt -&gt; en -&gt; de</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7251931924776773</v>
+        <v>0.6424549833932055</v>
       </c>
       <c r="C3" t="n">
-        <v>4.752190224454933</v>
-      </c>
-      <c r="D3" t="n">
-        <v>61.76296606406912</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; sv -&gt; de</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7262416235619358</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4.735488320271665</v>
-      </c>
-      <c r="D4" t="n">
-        <v>61.69778901423597</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; it -&gt; de</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7222638119306959</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4.764452767940378</v>
-      </c>
-      <c r="D5" t="n">
-        <v>62.31882412008308</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; es -&gt; sv -&gt; de</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.7161351345993449</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4.808970691628242</v>
-      </c>
-      <c r="D6" t="n">
-        <v>62.87608977081511</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; es -&gt; it -&gt; de</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.7108329624973082</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4.847730880585513</v>
-      </c>
-      <c r="D7" t="n">
-        <v>63.56382896127109</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; sv -&gt; it -&gt; de</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.7130036902668052</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.815399958194016</v>
-      </c>
-      <c r="D8" t="n">
-        <v>63.05716658823346</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>en -&gt; es -&gt; sv -&gt; it -&gt; de</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.7077072390922946</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4.855580036601012</v>
-      </c>
-      <c r="D9" t="n">
-        <v>63.68697442901672</v>
+        <v>4.113013400413599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cosine Similarity</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Euclidean Distance</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>es -&gt; sv</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.6813183323822003</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.425458745652767</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>es -&gt; it -&gt; sv</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.6650063280763135</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.505415393369554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Showing generated sentences with the metrics
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -459,10 +459,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7458308217580214</v>
+        <v>0.7592708010895827</v>
       </c>
       <c r="C2" t="n">
-        <v>3.608247796187873</v>
+        <v>4.143796545088468</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7253818860884673</v>
+        <v>0.7471509977842862</v>
       </c>
       <c r="C3" t="n">
-        <v>3.72803316185625</v>
+        <v>4.229964492103247</v>
       </c>
     </row>
   </sheetData>
@@ -512,27 +512,27 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>en -&gt; sv</t>
+          <t>en -&gt; de</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.770321545661382</v>
+        <v>0.749783041539854</v>
       </c>
       <c r="C2" t="n">
-        <v>4.096113994901942</v>
+        <v>4.820215035038566</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>en -&gt; de -&gt; sv</t>
+          <t>en -&gt; sv -&gt; de</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7507004719405196</v>
+        <v>0.737107234633723</v>
       </c>
       <c r="C3" t="n">
-        <v>4.223161091188399</v>
+        <v>4.912853220126173</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +573,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7458308217580214</v>
+        <v>0.7592708010895827</v>
       </c>
       <c r="C2" t="n">
-        <v>3.608247796187873</v>
+        <v>4.143796545088468</v>
       </c>
     </row>
     <row r="3">
@@ -586,10 +586,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7183457890793921</v>
+        <v>0.7323715599868168</v>
       </c>
       <c r="C3" t="n">
-        <v>3.794852705933903</v>
+        <v>4.375050645321163</v>
       </c>
     </row>
   </sheetData>
@@ -630,10 +630,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7458308217580214</v>
+        <v>0.7592708010895827</v>
       </c>
       <c r="C2" t="n">
-        <v>3.608247796187873</v>
+        <v>4.143796545088468</v>
       </c>
     </row>
     <row r="3">
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7183457890793921</v>
+        <v>0.7323715599868168</v>
       </c>
       <c r="C3" t="n">
-        <v>3.794852705933903</v>
+        <v>4.375050645321163</v>
       </c>
     </row>
   </sheetData>
@@ -687,10 +687,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6468203826557445</v>
+        <v>0.668403364983767</v>
       </c>
       <c r="C2" t="n">
-        <v>4.090183607972863</v>
+        <v>4.698783337542025</v>
       </c>
     </row>
     <row r="3">
@@ -700,10 +700,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6408274795095872</v>
+        <v>0.6620158784065271</v>
       </c>
       <c r="C3" t="n">
-        <v>4.115533117946701</v>
+        <v>4.732067402108964</v>
       </c>
     </row>
   </sheetData>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6468203826557445</v>
+        <v>0.668403364983767</v>
       </c>
       <c r="C2" t="n">
-        <v>4.090183607972863</v>
+        <v>4.698783337542025</v>
       </c>
     </row>
     <row r="3">
@@ -757,10 +757,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6335706796193548</v>
+        <v>0.6537497597011482</v>
       </c>
       <c r="C3" t="n">
-        <v>4.161656408540026</v>
+        <v>4.785809072147154</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7002179222798097</v>
+        <v>0.7066478643152803</v>
       </c>
       <c r="C2" t="n">
-        <v>4.79146594788603</v>
+        <v>5.405672186625698</v>
       </c>
     </row>
     <row r="3">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6786196424960104</v>
+        <v>0.6900929110843625</v>
       </c>
       <c r="C3" t="n">
-        <v>4.928405639552862</v>
+        <v>5.535204230993649</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +858,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7002179222798097</v>
+        <v>0.7066478643152803</v>
       </c>
       <c r="C2" t="n">
-        <v>4.79146594788603</v>
+        <v>5.405672186625698</v>
       </c>
     </row>
     <row r="3">
@@ -871,10 +871,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6880685322299915</v>
+        <v>0.6993193104625874</v>
       </c>
       <c r="C3" t="n">
-        <v>4.861872253650227</v>
+        <v>5.459112877717812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding BLEU score for single sentences
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Study case 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Study case 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Study case 3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Study case 4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Experiment 1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Experiment 2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Experiment 3" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Experiment 4" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Study case 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Study case 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Study case 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Study case 4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment 4" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,10 +459,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7592708010895827</v>
+        <v>0.75784908686924</v>
       </c>
       <c r="C2" t="n">
-        <v>4.143796545088468</v>
+        <v>3.928147304886926</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7471509977842862</v>
+        <v>0.7452189676354882</v>
       </c>
       <c r="C3" t="n">
-        <v>4.229964492103247</v>
+        <v>4.014194655748607</v>
       </c>
     </row>
   </sheetData>
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.749783041539854</v>
+        <v>0.7486132925533111</v>
       </c>
       <c r="C2" t="n">
-        <v>4.820215035038566</v>
+        <v>4.646439359915873</v>
       </c>
     </row>
     <row r="3">
@@ -529,10 +529,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.737107234633723</v>
+        <v>0.7341723396478861</v>
       </c>
       <c r="C3" t="n">
-        <v>4.912853220126173</v>
+        <v>4.742345045752013</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +573,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7592708010895827</v>
+        <v>0.75784908686924</v>
       </c>
       <c r="C2" t="n">
-        <v>4.143796545088468</v>
+        <v>3.928147304886926</v>
       </c>
     </row>
     <row r="3">
@@ -586,10 +586,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7323715599868168</v>
+        <v>0.7274824667297396</v>
       </c>
       <c r="C3" t="n">
-        <v>4.375050645321163</v>
+        <v>4.177093172467385</v>
       </c>
     </row>
   </sheetData>
@@ -630,10 +630,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7592708010895827</v>
+        <v>0.75784908686924</v>
       </c>
       <c r="C2" t="n">
-        <v>4.143796545088468</v>
+        <v>3.928147304886926</v>
       </c>
     </row>
     <row r="3">
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7323715599868168</v>
+        <v>0.7274824667297396</v>
       </c>
       <c r="C3" t="n">
-        <v>4.375050645321163</v>
+        <v>4.177093172467385</v>
       </c>
     </row>
   </sheetData>
@@ -687,10 +687,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.668403364983767</v>
+        <v>0.6624752232246374</v>
       </c>
       <c r="C2" t="n">
-        <v>4.698783337542025</v>
+        <v>4.462123810427518</v>
       </c>
     </row>
     <row r="3">
@@ -700,10 +700,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6620158784065271</v>
+        <v>0.6560882265792992</v>
       </c>
       <c r="C3" t="n">
-        <v>4.732067402108964</v>
+        <v>4.493955455642348</v>
       </c>
     </row>
   </sheetData>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.668403364983767</v>
+        <v>0.6624752232246374</v>
       </c>
       <c r="C2" t="n">
-        <v>4.698783337542025</v>
+        <v>4.462123810427518</v>
       </c>
     </row>
     <row r="3">
@@ -757,10 +757,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6537497597011482</v>
+        <v>0.6472810699802006</v>
       </c>
       <c r="C3" t="n">
-        <v>4.785809072147154</v>
+        <v>4.550112781227658</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7066478643152803</v>
+        <v>0.7070534090477629</v>
       </c>
       <c r="C2" t="n">
-        <v>5.405672186625698</v>
+        <v>5.180111994054941</v>
       </c>
     </row>
     <row r="3">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6900929110843625</v>
+        <v>0.6886481381166791</v>
       </c>
       <c r="C3" t="n">
-        <v>5.535204230993649</v>
+        <v>5.316211754647637</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +858,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7066478643152803</v>
+        <v>0.7070534090477629</v>
       </c>
       <c r="C2" t="n">
-        <v>5.405672186625698</v>
+        <v>5.180111994054941</v>
       </c>
     </row>
     <row r="3">
@@ -871,10 +871,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6993193104625874</v>
+        <v>0.698739271031948</v>
       </c>
       <c r="C3" t="n">
-        <v>5.459112877717812</v>
+        <v>5.233174198540799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated new grouped results | Commented BLEU
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -459,10 +459,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.75784908686924</v>
+        <v>0.7610360199449046</v>
       </c>
       <c r="C2" t="n">
-        <v>3.928147304886926</v>
+        <v>4.187896660234053</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7452189676354882</v>
+        <v>0.7488193612614225</v>
       </c>
       <c r="C3" t="n">
-        <v>4.014194655748607</v>
+        <v>4.274803858309955</v>
       </c>
     </row>
   </sheetData>
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7486132925533111</v>
+        <v>0.7512306351975814</v>
       </c>
       <c r="C2" t="n">
-        <v>4.646439359915873</v>
+        <v>4.850476179074347</v>
       </c>
     </row>
     <row r="3">
@@ -529,10 +529,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7341723396478861</v>
+        <v>0.73764237446588</v>
       </c>
       <c r="C3" t="n">
-        <v>4.742345045752013</v>
+        <v>4.951251305266382</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +573,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.75784908686924</v>
+        <v>0.7610360199449046</v>
       </c>
       <c r="C2" t="n">
-        <v>3.928147304886926</v>
+        <v>4.187896660234053</v>
       </c>
     </row>
     <row r="3">
@@ -586,10 +586,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7274824667297396</v>
+        <v>0.7355651945656037</v>
       </c>
       <c r="C3" t="n">
-        <v>4.177093172467385</v>
+        <v>4.411217825065794</v>
       </c>
     </row>
   </sheetData>
@@ -630,10 +630,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.75784908686924</v>
+        <v>0.7610360199449046</v>
       </c>
       <c r="C2" t="n">
-        <v>3.928147304886926</v>
+        <v>4.187896660234053</v>
       </c>
     </row>
     <row r="3">
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7274824667297396</v>
+        <v>0.7355651945656037</v>
       </c>
       <c r="C3" t="n">
-        <v>4.177093172467385</v>
+        <v>4.411217825065794</v>
       </c>
     </row>
   </sheetData>
@@ -687,10 +687,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6624752232246374</v>
+        <v>0.6720536429424536</v>
       </c>
       <c r="C2" t="n">
-        <v>4.462123810427518</v>
+        <v>4.727530209210354</v>
       </c>
     </row>
     <row r="3">
@@ -700,10 +700,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6560882265792992</v>
+        <v>0.665094505510461</v>
       </c>
       <c r="C3" t="n">
-        <v>4.493955455642348</v>
+        <v>4.762326107438171</v>
       </c>
     </row>
   </sheetData>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6624752232246374</v>
+        <v>0.6720536429424536</v>
       </c>
       <c r="C2" t="n">
-        <v>4.462123810427518</v>
+        <v>4.727530209210354</v>
       </c>
     </row>
     <row r="3">
@@ -757,10 +757,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6472810699802006</v>
+        <v>0.6572713830079461</v>
       </c>
       <c r="C3" t="n">
-        <v>4.550112781227658</v>
+        <v>4.815911196452968</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7070534090477629</v>
+        <v>0.7082380710354689</v>
       </c>
       <c r="C2" t="n">
-        <v>5.180111994054941</v>
+        <v>5.442023715745888</v>
       </c>
     </row>
     <row r="3">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6886481381166791</v>
+        <v>0.6920513250057071</v>
       </c>
       <c r="C3" t="n">
-        <v>5.316211754647637</v>
+        <v>5.569715858163367</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +858,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7070534090477629</v>
+        <v>0.7082380710354689</v>
       </c>
       <c r="C2" t="n">
-        <v>5.180111994054941</v>
+        <v>5.442023715745888</v>
       </c>
     </row>
     <row r="3">
@@ -871,10 +871,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.698739271031948</v>
+        <v>0.7010033836736442</v>
       </c>
       <c r="C3" t="n">
-        <v>5.233174198540799</v>
+        <v>5.494419528748598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>